<commit_message>
Split Course Code and Level on Summer Reporting File Spec
</commit_message>
<xml_diff>
--- a/api/src/test/resources/summer-reporting-invalid-MiddleName.xlsx
+++ b/api/src/test/resources/summer-reporting-invalid-MiddleName.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BAE0A7-C261-B148-A08D-FE9CD3B682AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB16271-926F-4147-82D2-1D25689E8D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="2200" windowWidth="21600" windowHeight="11300" xr2:uid="{9568818F-0947-4E3C-A15C-8486CBB48021}"/>
+    <workbookView xWindow="7095" yWindow="-10065" windowWidth="17250" windowHeight="10485" xr2:uid="{9568818F-0947-4E3C-A15C-8486CBB48021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>PEN</t>
   </si>
@@ -48,9 +48,6 @@
     <t>School Code</t>
   </si>
   <si>
-    <t>ENST 12</t>
-  </si>
-  <si>
     <t>Legal Middle Name</t>
   </si>
   <si>
@@ -72,20 +69,26 @@
     <t>Birthdate</t>
   </si>
   <si>
-    <t>Ministry Course Code and Level</t>
-  </si>
-  <si>
     <t>Final Percent</t>
   </si>
   <si>
     <t>Credits</t>
+  </si>
+  <si>
+    <t>Ministry Course Code</t>
+  </si>
+  <si>
+    <t>ENST</t>
+  </si>
+  <si>
+    <t>Ministry Course Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,23 +466,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187FDB52-F378-4ED2-BE59-01F37DC80983}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="17.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.5" style="3" customWidth="1"/>
+    <col min="3" max="5" width="17.44140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="13.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="8.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="43.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -490,31 +493,34 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="16.8">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -525,7 +531,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -534,22 +540,25 @@
         <v>20030516</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3">
         <v>202508</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>72</v>
       </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="3">
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -560,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -569,22 +578,25 @@
         <v>20030516</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3">
         <v>202508</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>72</v>
       </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -595,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -604,18 +616,21 @@
         <v>20030516</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3">
         <v>202508</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>72</v>
       </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="3">
         <v>4</v>
       </c>
     </row>

</xml_diff>